<commit_message>
Initialize mode split in Excel
</commit_message>
<xml_diff>
--- a/Data/init_mode_fuel_mix.xlsx
+++ b/Data/init_mode_fuel_mix.xlsx
@@ -1,32 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\egbertrv\Documents\GitHub\AIM_Norwegian_Freight_Model\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308E9F18-DE86-428D-BCD6-F0B59E980C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{308E9F18-DE86-428D-BCD6-F0B59E980C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8988841C-C501-42C3-934A-FFD86E431F2E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13800" yWindow="0" windowWidth="30345" windowHeight="23400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InitMix" sheetId="1" r:id="rId1"/>
-    <sheet name="MaturityScenariosAim" sheetId="2" r:id="rId2"/>
+    <sheet name="InitModeMix" sheetId="3" r:id="rId2"/>
+    <sheet name="MaturityScenariosAim" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="58">
   <si>
     <t>Mode</t>
   </si>
@@ -188,6 +200,18 @@
   </si>
   <si>
     <t>2026</t>
+  </si>
+  <si>
+    <t>https://www.toi.no/publikasjoner/grunnprognoser-for-godstransport-til-ntp-2018-2027-article33084-8.html</t>
+  </si>
+  <si>
+    <t>transport work (GTonnesKM)</t>
+  </si>
+  <si>
+    <t>Share</t>
+  </si>
+  <si>
+    <t>a too high share makes the model infeasible!</t>
   </si>
 </sst>
 </file>
@@ -359,6 +383,59 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>600938</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>105385</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01C517BB-75C6-4423-BECF-7562F6ECC5F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5391150" y="304800"/>
+          <a:ext cx="6182588" cy="4372585"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F48FEFFB-DFB6-47E1-B14A-80366FBE70B9}" name="Table1" displayName="Table1" ref="A1:D18" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:D18" xr:uid="{F48FEFFB-DFB6-47E1-B14A-80366FBE70B9}"/>
@@ -373,6 +450,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{233621A8-ACA8-4442-A992-6D0EF8235047}" name="Table3" displayName="Table3" ref="A1:C4" totalsRowShown="0">
+  <autoFilter ref="A1:C4" xr:uid="{233621A8-ACA8-4442-A992-6D0EF8235047}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{C240EB14-677E-493D-9CFA-088B455390D8}" name="Mode"/>
+    <tableColumn id="2" xr3:uid="{EE87F422-5D7B-4D49-8DD8-BA7C876C85B0}" name="transport work (GTonnesKM)"/>
+    <tableColumn id="3" xr3:uid="{679387ED-EEE4-49BB-9CF6-27C1FC31AF64}" name="Share">
+      <calculatedColumnFormula>B2/SUM($B$2:$B$4)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC2AF784-BCCF-4682-9727-DB3F7AC9F803}" name="Table2" displayName="Table2" ref="A1:H460" totalsRowShown="0">
   <autoFilter ref="A1:H460" xr:uid="{FC2AF784-BCCF-4682-9727-DB3F7AC9F803}">
     <filterColumn colId="0">
@@ -660,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,6 +761,8 @@
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -699,15 +792,9 @@
       <c r="D2" s="6">
         <v>100</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="3">
-        <v>100</v>
-      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -722,15 +809,9 @@
       <c r="D3" s="6">
         <v>0.5</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -745,15 +826,8 @@
       <c r="D4" s="6">
         <v>0.5</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0</v>
-      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -768,15 +842,9 @@
       <c r="D5" s="6">
         <v>5</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" s="3">
-        <v>5</v>
-      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -791,15 +859,9 @@
       <c r="D6" s="8">
         <v>0.5</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0</v>
-      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -814,15 +876,8 @@
       <c r="D7" s="10">
         <v>20</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="3">
-        <v>100</v>
-      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -837,15 +892,9 @@
       <c r="D8" s="10">
         <v>80</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8" s="3">
-        <v>100</v>
-      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -860,15 +909,9 @@
       <c r="D9" s="10">
         <v>10</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L9" s="3">
-        <v>10</v>
-      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -883,15 +926,9 @@
       <c r="D10" s="10">
         <v>0</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L10" s="3">
-        <v>0</v>
-      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -906,15 +943,9 @@
       <c r="D11" s="10">
         <v>0</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11" s="3">
-        <v>0</v>
-      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -929,15 +960,9 @@
       <c r="D12" s="10">
         <v>0</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="3">
-        <v>0</v>
-      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
@@ -952,15 +977,9 @@
       <c r="D13" s="14">
         <v>0</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L13" s="3">
-        <v>0</v>
-      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -975,15 +994,9 @@
       <c r="D14" s="12">
         <v>25</v>
       </c>
-      <c r="J14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L14" s="3">
-        <v>100</v>
-      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -998,18 +1011,9 @@
       <c r="D15" s="12">
         <v>80</v>
       </c>
-      <c r="F15" t="s">
-        <v>50</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L15" s="3">
-        <v>100</v>
-      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
@@ -1024,15 +1028,9 @@
       <c r="D16" s="12">
         <v>0</v>
       </c>
-      <c r="J16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L16" s="3">
-        <v>0</v>
-      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
@@ -1047,15 +1045,9 @@
       <c r="D17" s="12">
         <v>0</v>
       </c>
-      <c r="J17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L17" s="3">
-        <v>0</v>
-      </c>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
@@ -1070,15 +1062,12 @@
       <c r="D18" s="12">
         <v>0</v>
       </c>
-      <c r="J18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L18" s="3">
-        <v>0</v>
-      </c>
+      <c r="G18" t="s">
+        <v>50</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1090,6 +1079,78 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DE2A93-1896-459E-B2B3-A798F57F27DE}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="C2">
+        <f>B2/SUM($B$2:$B$4)</f>
+        <v>0.453125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>18.5</v>
+      </c>
+      <c r="C3" s="2">
+        <f>B3/SUM($B$2:$B$4)</f>
+        <v>0.48177083333333337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>2.5</v>
+      </c>
+      <c r="C4" s="2">
+        <f>B4/SUM($B$2:$B$4)</f>
+        <v>6.5104166666666671E-2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECAB6340-114B-49EA-A238-956B6E05C14E}">
   <dimension ref="A1:H460"/>
   <sheetViews>

</xml_diff>

<commit_message>
added Sea - MGO/HFO; updated accordingly
</commit_message>
<xml_diff>
--- a/Data/init_mode_fuel_mix.xlsx
+++ b/Data/init_mode_fuel_mix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\STraM_ntnu_development\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruben\GitHub\STraM_ntnu_development\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7842C012-4A81-4BF5-B4F2-9B44F3A4E362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C21AA4-C511-4EB5-9F03-7D7E0479F350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="init_mode_mix" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>Mode</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>Source for init_mode_mix: https://www.toi.no/publikasjoner/grunnprognoser-for-godstransport-til-ntp-2018-2027-article33084-8.html, see table below</t>
+  </si>
+  <si>
+    <t>MGO</t>
+  </si>
+  <si>
+    <t>HFO</t>
   </si>
 </sst>
 </file>
@@ -477,13 +483,13 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -506,7 +512,7 @@
         <v>0.453125</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -518,7 +524,7 @@
         <v>0.48177083333333337</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -537,21 +543,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D387E51-82CD-4762-B34F-6876BC940211}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -569,7 +575,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -583,7 +589,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -597,7 +603,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -611,7 +617,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -625,7 +631,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -639,7 +645,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -653,7 +659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -667,7 +673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -675,13 +681,13 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -689,13 +695,13 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -703,13 +709,13 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -717,9 +723,23 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>0</v>
       </c>
     </row>
@@ -733,31 +753,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9367BA79-D9B7-440E-87A5-AFAC1F2C8F4B}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="132.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="132.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
updated sea fuel mix
</commit_message>
<xml_diff>
--- a/Data/init_mode_fuel_mix.xlsx
+++ b/Data/init_mode_fuel_mix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruben\GitHub\STraM_ntnu_development\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C21AA4-C511-4EB5-9F03-7D7E0479F350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9588D90C-5460-4AFE-BD63-3EC0706EFCEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4824" yWindow="12" windowWidth="23040" windowHeight="12120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="init_mode_mix" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>Mode</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>HFO</t>
+  </si>
+  <si>
+    <t>Other source for init mode mix: https://dokumen.tips/documents/teknisk-vurdering-av-skip-og-av-infrastruktur-for-forsyning-av-drivstoff-.html</t>
+  </si>
+  <si>
+    <t>Split HFO/MGO based on figure 5-2 in source above</t>
   </si>
 </sst>
 </file>
@@ -546,7 +552,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,7 +690,7 @@
         <v>19</v>
       </c>
       <c r="D9">
-        <v>100</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -698,7 +704,7 @@
         <v>20</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -751,10 +757,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9367BA79-D9B7-440E-87A5-AFAC1F2C8F4B}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,6 +788,16 @@
         <v>17</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Updates to mode init and HFO cap
- The initial rail infrastructure allows 7GTONNES. This is much more than the initial split that we estimated. I suggest to remove the modal split initialization for rail, and rather enforce something for sea and road.
- Usage of HFO cannot increase over time.
</commit_message>
<xml_diff>
--- a/Data/init_mode_fuel_mix.xlsx
+++ b/Data/init_mode_fuel_mix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruben\GitHub\STraM_ntnu_development\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/STraM_ntnu_development/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE16982-A2F3-4D0A-B63B-7470077C8C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{3AE16982-A2F3-4D0A-B63B-7470077C8C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98E19C00-ABDD-42A4-803B-E0B3E212CC09}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="3840" windowWidth="23040" windowHeight="12120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="init_mode_mix" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>Mode</t>
   </si>
@@ -107,13 +107,25 @@
   </si>
   <si>
     <t>Split HFO/MGO based on figure 5-2 in source above</t>
+  </si>
+  <si>
+    <t>ShareCalc</t>
+  </si>
+  <si>
+    <t>The shares in the model should be at least as big , as the ones denoted here</t>
+  </si>
+  <si>
+    <t>maybe we have increased the shares by including sweden?</t>
+  </si>
+  <si>
+    <t>0.01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +135,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -150,10 +170,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,19 +504,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{742911F6-D010-432D-A1E8-3751DC9F8F22}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,45 +526,66 @@
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>17.399999999999999</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2">
         <f>B2/SUM($B$2:$B$4)</f>
         <v>0.453125</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
         <v>18.5</v>
       </c>
-      <c r="C3" s="2">
-        <f t="shared" ref="C3:C4" si="0">B3/SUM($B$2:$B$4)</f>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2">
+        <f>B3/SUM($B$2:$B$4)</f>
         <v>0.48177083333333337</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
         <v>2.5</v>
       </c>
-      <c r="C4" s="2">
-        <f t="shared" si="0"/>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2">
+        <f>B4/SUM($B$2:$B$4)</f>
         <v>6.5104166666666671E-2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -551,19 +593,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D387E51-82CD-4762-B34F-6876BC940211}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -581,7 +623,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -595,7 +637,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -609,7 +651,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -623,7 +665,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -637,7 +679,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -651,7 +693,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -665,7 +707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -679,7 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -693,7 +735,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -707,7 +749,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -721,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -735,7 +777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -763,37 +805,37 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="132.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="132.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>

</xml_diff>